<commit_message>
Revisão dos diagramas v2
Foram alterados os diagramas de Caso de uso e do Diagrama de Classe, prints
</commit_message>
<xml_diff>
--- a/Documentação/Sistema  Documentação/Requisitos/Requisitos P.i.xlsx
+++ b/Documentação/Sistema  Documentação/Requisitos/Requisitos P.i.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karina\Downloads\P.I ( Projeto Integrador)\P.I 2º Semmestre\Sistema  Documentação\Requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Karina\Documents\Fatec - DSM\P.I ( Projeto Integrador)\P.I 2º Semmestre\Sistema  Documentação\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6000" windowWidth="17256" windowHeight="5772"/>
+    <workbookView minimized="1" xWindow="0" yWindow="6600" windowWidth="17256" windowHeight="5772"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -134,9 +134,6 @@
     <t>Desejável</t>
   </si>
   <si>
-    <t>Usuários do sistema, seja o principal ( advogada) ou clientes, devem ter acesso às suas respectiva  pendências  (pagas  ou a  pagar),  constando como efetuada ou atrasada.</t>
-  </si>
-  <si>
     <t>Requisitos Não Funcionais</t>
   </si>
   <si>
@@ -192,6 +189,9 @@
   </si>
   <si>
     <t xml:space="preserve">Backup diario após o expediente </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Usuários do sistema, seja o principal ( advogada) ou clientes, devem ter acesso às suas respectiva  pendências  (pagas  ou a  pagar),  constando como efetuada ou atrasada. </t>
   </si>
 </sst>
 </file>
@@ -358,12 +358,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -384,15 +393,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24:H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,17 +691,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="26"/>
-      <c r="F1" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="29"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="F1" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -727,18 +727,18 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-      <c r="F3" s="21" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="26"/>
+      <c r="F3" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -761,7 +761,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>26</v>
@@ -774,16 +774,16 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23"/>
-      <c r="F6" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="26"/>
+      <c r="F6" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
       <c r="I6" s="8" t="s">
         <v>14</v>
       </c>
@@ -799,7 +799,7 @@
     </row>
     <row r="8" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>5</v>
@@ -808,7 +808,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>15</v>
@@ -821,16 +821,16 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="22"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="20"/>
-      <c r="F9" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="F9" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
       <c r="I9" s="8" t="s">
         <v>16</v>
       </c>
@@ -846,7 +846,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>32</v>
@@ -858,7 +858,7 @@
         <v>23</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>0</v>
@@ -868,16 +868,16 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="32"/>
-      <c r="F12" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
+      <c r="A12" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="21"/>
+      <c r="F12" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
       <c r="I12" s="8" t="s">
         <v>17</v>
       </c>
@@ -893,7 +893,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>4</v>
@@ -915,16 +915,16 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="22"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="20"/>
-      <c r="F15" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
+      <c r="F15" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
       <c r="I15" s="17" t="s">
         <v>20</v>
       </c>
@@ -962,16 +962,16 @@
       </c>
     </row>
     <row r="18" spans="1:9" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="22"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="20"/>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
       <c r="I18" s="17" t="s">
         <v>20</v>
       </c>
@@ -990,7 +990,7 @@
         <v>8</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H20" s="11" t="s">
         <v>3</v>
@@ -1000,11 +1000,11 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F21" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
+      <c r="F21" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
       <c r="I21" s="8" t="s">
         <v>11</v>
       </c>
@@ -1021,37 +1021,37 @@
       <c r="C23" s="6"/>
       <c r="D23" s="1"/>
       <c r="F23" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="H23" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>54</v>
       </c>
       <c r="I23" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="1"/>
-      <c r="F24" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
+      <c r="F24" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
       <c r="I24" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
       <c r="F25" s="2"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1064,9 +1064,9 @@
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
       <c r="I27" s="19"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1086,12 +1086,12 @@
       <c r="I29" s="6"/>
     </row>
     <row r="30" spans="1:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-      <c r="H30" s="30"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
       <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -1110,9 +1110,9 @@
       <c r="I32" s="6"/>
     </row>
     <row r="33" spans="6:9" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
       <c r="I33" s="19"/>
     </row>
     <row r="34" spans="6:9" x14ac:dyDescent="0.3">
@@ -1123,6 +1123,15 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="F24:H24"/>
     <mergeCell ref="A30:C30"/>
@@ -1136,15 +1145,6 @@
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>